<commit_message>
Added 300 influencer photos & placeholders.
</commit_message>
<xml_diff>
--- a/Influencers .xlsx
+++ b/Influencers .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Kourakos\AMG Media\Presentations\Creator Network\Landing Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A0194F-3AB6-4B6D-892D-1F19A6B80C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455BBC38-27E2-47FE-B8F8-E362AFFDC028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6409,7 +6409,7 @@
   <dimension ref="A1:Z562"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>